<commit_message>
productdetails test class has been tested using dataproviders and pojo and excel apachepoi
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/OpenCartTestData.xlsx
+++ b/src/main/resources/TestData/OpenCartTestData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harit\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harit\Javasessions\OpenCartAutomation\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1471390D-7BEA-410C-9841-9397211BF0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0266A9D7-0DBA-4CAD-90BB-7F011F8576C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C2D7037-60B9-4A04-A96A-E0B9FBE8DDB7}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4C2D7037-60B9-4A04-A96A-E0B9FBE8DDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
+    <sheet name="productinfo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>firstname</t>
   </si>
@@ -93,12 +94,54 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>searchstring</t>
+  </si>
+  <si>
+    <t>productSelected</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Reward Points</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Ex Tax</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>samsung</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Tab 10.1</t>
+  </si>
+  <si>
+    <t>SAM1</t>
+  </si>
+  <si>
+    <t>Pre-Order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +169,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,12 +207,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D51A57-DD79-4B0B-8BD0-6DAF129BB3BB}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -589,4 +640,85 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C73218-3895-44E5-A4B8-46B0F7A0B562}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="11.05859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.76171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.64453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.87890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.76171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.76171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="5">
+        <v>241.99</v>
+      </c>
+      <c r="G2" s="5">
+        <v>199.99</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>